<commit_message>
footer only for prive
</commit_message>
<xml_diff>
--- a/now.xlsx
+++ b/now.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>No</t>
   </si>
@@ -40,73 +40,64 @@
     <t>TVA CHE 110.257.937</t>
   </si>
   <si>
-    <t>OFFRE N: base</t>
-  </si>
-  <si>
-    <t>Genève, le 18/04/2021</t>
-  </si>
-  <si>
-    <t>CONCERNE: base</t>
+    <t>OFFRE N: offre</t>
+  </si>
+  <si>
+    <t>Genève, le 01/05/2021</t>
+  </si>
+  <si>
+    <t>CONCERNE: concerne</t>
   </si>
   <si>
     <t xml:space="preserve">Adresse: </t>
   </si>
   <si>
-    <t>BASE REGIE}</t>
+    <t>Privé</t>
   </si>
   <si>
     <t xml:space="preserve">Contact: </t>
   </si>
   <si>
+    <t>Selon votre demande de devis No: devis</t>
+  </si>
+  <si>
     <t>Vos Contact: Admin</t>
   </si>
   <si>
     <t>PRÉPARATION</t>
   </si>
   <si>
-    <t>Divers &amp; mise en place</t>
-  </si>
-  <si>
-    <t>Pont-Roulant, hauteur de travail maximum 5m - Manutention, montage, ajustement, mise à disposition le temps des travaux, démontage et évacuation - En cas d'utilisation par une entreprise tiers, la modification du pont roulant est strictement interdites, nous déclinons toutes responsabilités en cas de modifications non autorisées</t>
-  </si>
-  <si>
-    <t>Démontage spécifique</t>
-  </si>
-  <si>
-    <t>Démontage et évacuation à la décharge des éléments électroménagers y compris taxes de recyclage</t>
-  </si>
-  <si>
-    <t>Démolition, sciage et mise en sac et manutention des armoires, y compris évacuation à la décharge et taxe de recyclage des déchets</t>
+    <t>Démolition</t>
+  </si>
+  <si>
+    <t>Dépose des divers bâtissages sanitaires - évacuation, y compris taxes de recyclage</t>
+  </si>
+  <si>
+    <t>Piquage du carrelage (hors désamiantage), mise en sac manutention et évacuation des gravats, y compris taxes de recyclage</t>
+  </si>
+  <si>
+    <t>Dépose d'un muret de baignoire - évacuation, y compris taxes de recyclage</t>
+  </si>
+  <si>
+    <t>Arrachage des plinthes, sciage, mise en sac, manutention, évacuation à la décharge et taxes de traitement des déchets</t>
+  </si>
+  <si>
+    <t>Arrachage du parquet, sciage, mise en sac, manutention, évacuation à la décharge et taxes de traitement des déchets</t>
+  </si>
+  <si>
+    <t>Enduisage des murs existants</t>
   </si>
   <si>
     <t>Sous-total</t>
   </si>
   <si>
-    <t>SECHE</t>
-  </si>
-  <si>
-    <t>Plafond</t>
-  </si>
-  <si>
-    <t>Préparation du support, rhabillage des fissures, masticage, divres</t>
-  </si>
-  <si>
-    <t>Murs</t>
-  </si>
-  <si>
-    <t>Grattage de la peinture équiaillée et du plâtre fusé jusqu'au support sain, mise en sac, évacuation et taxes de recyclage</t>
-  </si>
-  <si>
-    <t>Ouverture et traitement de fissures, lissage partiel et ponçage</t>
-  </si>
-  <si>
-    <t>Masticage divers et ponçage</t>
-  </si>
-  <si>
-    <t>Murs crépi</t>
-  </si>
-  <si>
-    <t>Application d'une couche d'accrochage pour plâtre</t>
+    <t>SANITAIRE</t>
+  </si>
+  <si>
+    <t>Raccordement évier de cuisine</t>
+  </si>
+  <si>
+    <t>Dépose existant, raccordement de batterie monotrou pour évier, siphon double pour évier, 1 robinet "Siduo" avec attente pour LV. Modification alimentations et écoulement. Position à définir selon plan de cuisine</t>
   </si>
   <si>
     <t>TOTAL H.T</t>
@@ -157,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,###0.##"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -171,13 +162,9 @@
     </font>
     <font>
       <b/>
-      <u/>
     </font>
     <font>
       <color rgb="FFFFFFFF"/>
-    </font>
-    <font>
-      <b/>
     </font>
     <font>
       <i/>
@@ -223,13 +210,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -626,7 +613,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G65"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -699,361 +686,300 @@
       </c>
       <c r="B16"/>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17"/>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="G20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>1</v>
-      </c>
-      <c r="B23" s="4" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C23" s="4">
-        <v>18</v>
-      </c>
-      <c r="D23" s="4">
-        <f>IF(C23 * G23 &lt;= 750, "bloc", "pc")</f>
-      </c>
-      <c r="E23" s="4">
-        <f>IF(C23 * G23 &lt;= 750, F23, G23)</f>
-      </c>
-      <c r="F23" s="4">
-        <f>MAX(C23 * G23, 750)</f>
-      </c>
-      <c r="G23" s="5">
-        <v>750</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3</v>
+      </c>
+      <c r="D24" s="4">
+        <f>IF(C24 * G24 &lt;= 500, "bloc", "bloc")</f>
+      </c>
+      <c r="E24" s="4">
+        <f>IF(C24 * G24 &lt;= 500, F24, G24)</f>
+      </c>
+      <c r="F24" s="4">
+        <f>CEILING(MAX(C24 * G24, 500), 0.05)</f>
+      </c>
+      <c r="G24" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>2</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="4">
-        <v>32</v>
-      </c>
-      <c r="D24" s="4">
-        <f>IF(C24 * G24 &lt;= 750, "bloc", "pc")</f>
-      </c>
-      <c r="E24" s="4">
-        <f>IF(C24 * G24 &lt;= 750, F24, G24)</f>
-      </c>
-      <c r="F24" s="4">
-        <f>MAX(C24 * G24, 750)</f>
-      </c>
-      <c r="G24" s="5">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="B25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4">
+        <f>IF(C25 * G25 &lt;= 150, "bloc", "en bloc")</f>
+      </c>
+      <c r="E25" s="4">
+        <f>IF(C25 * G25 &lt;= 150, F25, G25)</f>
+      </c>
+      <c r="F25" s="4">
+        <f>CEILING(MAX(C25 * G25, 150), 0.05)</f>
+      </c>
+      <c r="G25" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>3</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="4">
+        <v>3</v>
+      </c>
+      <c r="D26" s="4">
+        <f>IF(C26 * G26 &lt;= 150, "bloc", "pc")</f>
+      </c>
+      <c r="E26" s="4">
+        <f>IF(C26 * G26 &lt;= 150, F26, G26)</f>
+      </c>
+      <c r="F26" s="4">
+        <f>CEILING(MAX(C26 * G26, 150), 0.05)</f>
+      </c>
+      <c r="G26" s="5">
+        <v>150</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C27" s="4">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D27" s="4">
-        <f>IF(C27 * G27 &lt;= 0, "bloc", "en bloc")</f>
+        <f>IF(C27 * G27 &lt;= 50, "bloc", "ml")</f>
       </c>
       <c r="E27" s="4">
-        <f>IF(C27 * G27 &lt;= 0, F27, G27)</f>
+        <f>IF(C27 * G27 &lt;= 50, F27, G27)</f>
       </c>
       <c r="F27" s="4">
-        <f>MAX(C27 * G27, 0)</f>
+        <f>CEILING(MAX(C27 * G27, 50), 0.05)</f>
       </c>
       <c r="G27" s="5">
-        <v>350</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C28" s="4">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D28" s="4">
-        <f>IF(C28 * G28 &lt;= 0, "bloc", "pc")</f>
+        <f>IF(C28 * G28 &lt;= 150, "bloc", "m2")</f>
       </c>
       <c r="E28" s="4">
-        <f>IF(C28 * G28 &lt;= 0, F28, G28)</f>
+        <f>IF(C28 * G28 &lt;= 150, F28, G28)</f>
       </c>
       <c r="F28" s="4">
-        <f>MAX(C28 * G28, 0)</f>
+        <f>CEILING(MAX(C28 * G28, 150), 0.05)</f>
       </c>
       <c r="G28" s="5">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="7">
-        <f>SUM(F21:F28)</f>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>5</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>6</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4">
+        <v>3</v>
+      </c>
+      <c r="D31" s="4">
+        <f>IF(C31 * G31 &lt;= 0, "bloc", "undefined")</f>
+      </c>
+      <c r="E31" s="4">
+        <f>IF(C31 * G31 &lt;= 0, F31, G31)</f>
+      </c>
+      <c r="F31" s="4">
+        <f>CEILING(MAX(C31 * G31, 0), 0.05)</f>
+      </c>
+      <c r="G31" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="4">
-        <v>1</v>
-      </c>
-      <c r="D35" s="4">
-        <f>IF(C35 * G35 &lt;= 0, "bloc", "h")</f>
-      </c>
-      <c r="E35" s="4">
-        <f>IF(C35 * G35 &lt;= 0, F35, G35)</f>
-      </c>
-      <c r="F35" s="4">
-        <f>MAX(C35 * G35, 0)</f>
-      </c>
-      <c r="G35" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="7">
+        <f>CEILING(SUM(F22:F31), 0.05)</f>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C38" s="4">
         <v>3</v>
       </c>
       <c r="D38" s="4">
-        <f>IF(C38 * G38 &lt;= 0, "bloc", "h")</f>
+        <f>IF(C38 * G38 &lt;= 0, "bloc", "forfait")</f>
       </c>
       <c r="E38" s="4">
         <f>IF(C38 * G38 &lt;= 0, F38, G38)</f>
       </c>
       <c r="F38" s="4">
-        <f>MAX(C38 * G38, 0)</f>
+        <f>CEILING(MAX(C38 * G38, 0), 0.05)</f>
       </c>
       <c r="G38" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>7</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="4">
-        <v>5</v>
-      </c>
-      <c r="D39" s="4">
-        <f>IF(C39 * G39 &lt;= 0, "bloc", "h")</f>
-      </c>
-      <c r="E39" s="4">
-        <f>IF(C39 * G39 &lt;= 0, F39, G39)</f>
-      </c>
-      <c r="F39" s="4">
-        <f>MAX(C39 * G39, 0)</f>
-      </c>
-      <c r="G39" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
-        <v>8</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="4">
-        <v>5</v>
-      </c>
-      <c r="D40" s="4">
-        <f>IF(C40 * G40 &lt;= 0, "bloc", "h")</f>
-      </c>
-      <c r="E40" s="4">
-        <f>IF(C40 * G40 &lt;= 0, F40, G40)</f>
-      </c>
-      <c r="F40" s="4">
-        <f>MAX(C40 * G40, 0)</f>
-      </c>
-      <c r="G40" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <v>9</v>
-      </c>
-      <c r="B41" s="4" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="7">
+        <f>CEILING(SUM(F36:F38), 0.05)</f>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="4">
-        <v>5</v>
-      </c>
-      <c r="D41" s="4">
-        <f>IF(C41 * G41 &lt;= 0, "bloc", "h")</f>
-      </c>
-      <c r="E41" s="4">
-        <f>IF(C41 * G41 &lt;= 0, F41, G41)</f>
-      </c>
-      <c r="F41" s="4">
-        <f>MAX(C41 * G41, 0)</f>
-      </c>
-      <c r="G41" s="5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>10</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="4">
-        <v>2</v>
-      </c>
-      <c r="D44" s="4">
-        <f>IF(C44 * G44 &lt;= 0, "bloc", "m2")</f>
-      </c>
-      <c r="E44" s="4">
-        <f>IF(C44 * G44 &lt;= 0, F44, G44)</f>
-      </c>
-      <c r="F44" s="4">
-        <f>MAX(C44 * G44, 0)</f>
-      </c>
-      <c r="G44" s="5">
-        <v>8</v>
+      <c r="F44" s="7">
+        <f>=CEILING(SUM(F32,F39), 0.05)</f>
       </c>
     </row>
     <row r="45" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1070,181 +996,137 @@
         <v>6</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F45" s="7">
-        <f>SUM(F33:F44)</f>
-      </c>
-    </row>
-    <row r="50" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="6" t="s">
+        <f>F44*7.7%</f>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F47" s="7">
+        <f>F44+F45</f>
+      </c>
+    </row>
+    <row r="50" ht="100" customHeight="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F50" s="7">
-        <f>SUM(F29,F45)</f>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="6" t="s">
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="52" ht="60" customHeight="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F51" s="7">
-        <f>F50*7.7%</f>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="6" t="s">
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="55" ht="30" customHeight="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F53" s="7">
-        <f>F50+F51</f>
-      </c>
-    </row>
-    <row r="56" ht="100" customHeight="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="8" t="s">
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+    </row>
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-    </row>
-    <row r="58" ht="60" customHeight="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="8" t="s">
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
         <v>35</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-    </row>
-    <row r="61" ht="30" customHeight="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="9" t="s">
+      <c r="C59" t="s">
         <v>36</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="63" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="8" t="s">
+    </row>
+    <row r="63" ht="30" customHeight="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="65" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" ht="30" customHeight="1" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-    </row>
-    <row r="71" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="10"/>
-      <c r="F71" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="15">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B52:F52"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B57:F57"/>
     <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B65:F65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="7" fitToHeight="5"/>
   <headerFooter>
-    <oddHeader>94-undefined</oddHeader>
+    <oddHeader>95-undefined</oddHeader>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
not merge room titles
</commit_message>
<xml_diff>
--- a/now.xlsx
+++ b/now.xlsx
@@ -1106,7 +1106,7 @@
       <c r="F65" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="13">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A11:B11"/>
@@ -1114,8 +1114,6 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B35:F35"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B52:F52"/>
     <mergeCell ref="B55:F55"/>

</xml_diff>